<commit_message>
Fixed timing results to represent 40 byte string messages
</commit_message>
<xml_diff>
--- a/Implementation/Testing/Results/timings.xlsx
+++ b/Implementation/Testing/Results/timings.xlsx
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
-  <si>
-    <t>Named Pipes</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t xml:space="preserve">Run </t>
   </si>
@@ -33,7 +30,13 @@
     <t>Average</t>
   </si>
   <si>
-    <t>Mailslot</t>
+    <t>Named Pipes (40 Bytes)</t>
+  </si>
+  <si>
+    <t>Mailslot (40 Bytes)</t>
+  </si>
+  <si>
+    <t>Winsock (40 Bytes)</t>
   </si>
 </sst>
 </file>
@@ -369,17 +372,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -388,181 +394,260 @@
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
       <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>467445</v>
+        <v>1077617</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3">
-        <v>1142183</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>887315</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>2504495</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>581098</v>
+        <v>551269</v>
       </c>
       <c r="D4">
         <v>2</v>
       </c>
       <c r="E4">
-        <v>835587</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>864283</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>2651374</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>457251</v>
+        <v>780460</v>
       </c>
       <c r="D5">
         <v>3</v>
       </c>
       <c r="E5">
-        <v>721557</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>831811</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>2703858</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>572790</v>
+        <v>1119150</v>
       </c>
       <c r="D6">
         <v>4</v>
       </c>
       <c r="E6">
-        <v>866926</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1107823</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="H6">
+        <v>3002902</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>675492</v>
+        <v>1043634</v>
       </c>
       <c r="D7">
         <v>5</v>
       </c>
       <c r="E7">
-        <v>1139162</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>973781</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <v>2988554</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>773287</v>
+        <v>926584</v>
       </c>
       <c r="D8">
         <v>6</v>
       </c>
       <c r="E8">
-        <v>967363</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>899020</v>
+      </c>
+      <c r="G8">
+        <v>6</v>
+      </c>
+      <c r="H8">
+        <v>2392731</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>446678</v>
+        <v>1069687</v>
       </c>
       <c r="D9">
         <v>7</v>
       </c>
       <c r="E9">
-        <v>849558</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>819351</v>
+      </c>
+      <c r="G9">
+        <v>7</v>
+      </c>
+      <c r="H9">
+        <v>2601534</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>486324</v>
+        <v>1432920</v>
       </c>
       <c r="D10">
         <v>8</v>
       </c>
       <c r="E10">
-        <v>931492</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>844649</v>
+      </c>
+      <c r="G10">
+        <v>8</v>
+      </c>
+      <c r="H10">
+        <v>2953061</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>1268672</v>
+        <v>770265</v>
       </c>
       <c r="D11">
         <v>9</v>
       </c>
       <c r="E11">
-        <v>709853</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1049675</v>
+      </c>
+      <c r="G11">
+        <v>9</v>
+      </c>
+      <c r="H11">
+        <v>2869993</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>507469</v>
+        <v>917145</v>
       </c>
       <c r="D12">
         <v>10</v>
       </c>
       <c r="E12">
-        <v>936023</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>674737</v>
+      </c>
+      <c r="G12">
+        <v>10</v>
+      </c>
+      <c r="H12">
+        <v>2567551</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B13">
         <f>AVERAGE(B3:B12)</f>
-        <v>623650.6</v>
+        <v>968873.1</v>
       </c>
       <c r="D13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E13">
         <f>AVERAGE(E3:E12)</f>
-        <v>909970.4</v>
+        <v>895244.5</v>
+      </c>
+      <c r="G13" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13">
+        <f>AVERAGE(H3:H12)/2</f>
+        <v>1361802.65</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added results of Java sockets
</commit_message>
<xml_diff>
--- a/Implementation/Testing/Results/timings.xlsx
+++ b/Implementation/Testing/Results/timings.xlsx
@@ -18,8 +18,66 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="H13" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Divided by 2 to represent sending of 1 message (i.e. not echoed back)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K13" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Divided by 2 to represent sending of 1 message (i.e. not echoed back)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
   <si>
     <t xml:space="preserve">Run </t>
   </si>
@@ -38,12 +96,15 @@
   <si>
     <t>Winsock (40 Bytes)</t>
   </si>
+  <si>
+    <t>Java Sockets (40 Bytes)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -59,6 +120,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -371,19 +445,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.375" customWidth="1"/>
+    <col min="11" max="11" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -399,8 +474,13 @@
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -419,8 +499,14 @@
       <c r="H2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -439,8 +525,14 @@
       <c r="H3">
         <v>2504495</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>6751526</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -459,8 +551,14 @@
       <c r="H4">
         <v>2651374</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <v>5226476</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -479,8 +577,14 @@
       <c r="H5">
         <v>2703858</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <v>3</v>
+      </c>
+      <c r="K5">
+        <v>5336353</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -499,8 +603,14 @@
       <c r="H6">
         <v>3002902</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <v>4</v>
+      </c>
+      <c r="K6">
+        <v>5476813</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -519,8 +629,14 @@
       <c r="H7">
         <v>2988554</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <v>5</v>
+      </c>
+      <c r="K7">
+        <v>5819657</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -539,8 +655,14 @@
       <c r="H8">
         <v>2392731</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <v>6</v>
+      </c>
+      <c r="K8">
+        <v>5788695</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -559,8 +681,14 @@
       <c r="H9">
         <v>2601534</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <v>7</v>
+      </c>
+      <c r="K9">
+        <v>5524766</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -579,8 +707,14 @@
       <c r="H10">
         <v>2953061</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <v>8</v>
+      </c>
+      <c r="K10">
+        <v>8326795</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -599,8 +733,14 @@
       <c r="H11">
         <v>2869993</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <v>9</v>
+      </c>
+      <c r="K11">
+        <v>6031479</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -619,8 +759,14 @@
       <c r="H12">
         <v>2567551</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <v>10</v>
+      </c>
+      <c r="K12">
+        <v>5402429</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -642,14 +788,23 @@
         <f>AVERAGE(H3:H12)/2</f>
         <v>1361802.65</v>
       </c>
+      <c r="J13" t="s">
+        <v>2</v>
+      </c>
+      <c r="K13">
+        <f>AVERAGE(K3:K12)/2</f>
+        <v>2984249.45</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="G1:I1"/>
+    <mergeCell ref="J1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Message can now be accessed. Needs to be made more generic.
</commit_message>
<xml_diff>
--- a/Implementation/Testing/Results/timings.xlsx
+++ b/Implementation/Testing/Results/timings.xlsx
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
   <si>
     <t xml:space="preserve">Run </t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>Java Sockets (40 Bytes)</t>
+  </si>
+  <si>
+    <t>Memory Mapping (40 Bytes)</t>
   </si>
 </sst>
 </file>
@@ -446,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -796,8 +799,79 @@
         <v>2984249.45</v>
       </c>
     </row>
+    <row r="14" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
+    <mergeCell ref="A14:C14"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="G1:I1"/>

</xml_diff>

<commit_message>
Test programs - recorded some timings
</commit_message>
<xml_diff>
--- a/Implementation/Testing/Results/timings.xlsx
+++ b/Implementation/Testing/Results/timings.xlsx
@@ -452,7 +452,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -818,55 +818,89 @@
       <c r="A16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>90241</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>75516</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>80047</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>71363</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>74006</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>107610</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>7</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>114407</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>72873</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>89487</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>10</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>74383</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>2</v>
+      </c>
+      <c r="B26">
+        <f>AVERAGE(B16:B25)</f>
+        <v>84993.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>